<commit_message>
add verigen _V macro
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_module.xlsx
+++ b/Common/doc/verigen/media/instruction_module.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF28F20-CE97-4066-9FE3-138082419ABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F754CD2-93D4-46B0-8572-32811753AD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="13" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6000" yWindow="330" windowWidth="18390" windowHeight="15300" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -30,11 +30,12 @@
     <sheet name="get_port" sheetId="31" r:id="rId15"/>
     <sheet name="add_module" sheetId="32" r:id="rId16"/>
     <sheet name="get_module" sheetId="33" r:id="rId17"/>
-    <sheet name="i_set_param" sheetId="34" r:id="rId18"/>
-    <sheet name="i_get_param" sheetId="35" r:id="rId19"/>
-    <sheet name="i_set_port" sheetId="36" r:id="rId20"/>
-    <sheet name="i_get_port" sheetId="37" r:id="rId21"/>
-    <sheet name="i_is_valid" sheetId="38" r:id="rId22"/>
+    <sheet name="add_code" sheetId="39" r:id="rId18"/>
+    <sheet name="i_set_param" sheetId="34" r:id="rId19"/>
+    <sheet name="i_get_param" sheetId="35" r:id="rId20"/>
+    <sheet name="i_set_port" sheetId="36" r:id="rId21"/>
+    <sheet name="i_get_port" sheetId="37" r:id="rId22"/>
+    <sheet name="i_is_valid" sheetId="38" r:id="rId23"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="130">
   <si>
     <t>표현식</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -288,10 +289,6 @@
   </si>
   <si>
     <t>.code</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>module 코드 문자열</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -563,6 +560,39 @@
   </si>
   <si>
     <t>module_i 객체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>:add_code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자 코드 문장을 추가합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>String</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>module 의 추가된 코드 문자열 객체</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function module:add_code(s)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자 추가 코드</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>사용자 코드 추가합니다.
+이 코드들은 각 모듈 소스의 맨 마지막에 삽입되는 문장으로 포함됩니다. module.code(String) 객체에 추가되며, _V() 메크로 함수와 함께 유용하게 사용될 수 있습니다. 추가된 코드의 마지막 문자가 ';' 로 끝날 경우 자동으로 enter code가 삽입됩니다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -898,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1552F-D2B8-4AD9-9ECE-3CAF9162E459}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1066,35 +1096,46 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>122</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>45</v>
+        <v>123</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>57</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" t="s">
-        <v>58</v>
+      <c r="B18" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>
@@ -1123,7 +1164,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1139,7 +1180,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1147,7 +1188,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -1176,7 +1217,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1192,7 +1233,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1205,18 +1246,18 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" t="s">
         <v>81</v>
-      </c>
-      <c r="B5" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" t="s">
         <v>83</v>
-      </c>
-      <c r="B6" t="s">
-        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1245,7 +1286,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1253,7 +1294,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1261,7 +1302,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1298,7 +1339,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1306,7 +1347,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1314,15 +1355,15 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" t="s">
         <v>91</v>
-      </c>
-      <c r="B4" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1330,7 +1371,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1359,7 +1400,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1367,7 +1408,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1375,7 +1416,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1383,7 +1424,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1412,7 +1453,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1420,7 +1461,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="33" x14ac:dyDescent="0.3">
@@ -1428,7 +1469,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1436,7 +1477,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -1464,7 +1505,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1485,10 +1526,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="66" x14ac:dyDescent="0.3">
@@ -1496,7 +1537,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1511,7 +1552,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1525,7 +1566,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1541,7 +1582,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1549,7 +1590,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1560,6 +1601,58 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28113802-B713-49E4-A818-7E4C797F3E8E}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A772622C-72EA-4547-94FE-9EA66C7FB6BE}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1578,7 +1671,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1594,7 +1687,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1607,63 +1700,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F508A2DE-DD70-49F7-944A-ED879E70751B}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="55.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1760,6 +1800,59 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F508A2DE-DD70-49F7-944A-ED879E70751B}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F942EC-D9CE-4518-8AE9-9DD2A68C7F6E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1778,7 +1871,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1794,7 +1887,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1802,15 +1895,15 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B5" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -1820,7 +1913,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3433696-309F-48A2-94BE-A5A058FB822B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1839,7 +1932,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1847,7 +1940,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1855,7 +1948,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1863,7 +1956,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1873,11 +1966,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1D0C89-3871-4B99-A935-D12B0A533798}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1892,7 +1985,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1908,7 +2001,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1916,7 +2009,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -2013,7 +2106,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2029,7 +2122,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2065,7 +2158,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2081,7 +2174,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2089,7 +2182,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -2125,7 +2218,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2141,7 +2234,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2149,7 +2242,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -2185,7 +2278,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2201,15 +2294,15 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
         <v>67</v>
-      </c>
-      <c r="B5" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2254,7 +2347,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2270,7 +2363,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2299,7 +2392,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2315,15 +2408,15 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
         <v>74</v>
-      </c>
-      <c r="B4" t="s">
-        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
verigen : add module.apply_code
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_module.xlsx
+++ b/Common/doc/verigen/media/instruction_module.xlsx
@@ -8,34 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F754CD2-93D4-46B0-8572-32811753AD3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276A410C-B576-4CBD-976C-2E3B7DCB086E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="330" windowWidth="18390" windowHeight="15300" firstSheet="13" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6000" yWindow="330" windowWidth="18390" windowHeight="15300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
     <sheet name="summary_i" sheetId="7" r:id="rId2"/>
     <sheet name="new" sheetId="1" r:id="rId3"/>
     <sheet name="make_code" sheetId="8" r:id="rId4"/>
-    <sheet name="find" sheetId="9" r:id="rId5"/>
-    <sheet name="is_valid" sheetId="10" r:id="rId6"/>
-    <sheet name="set_inception" sheetId="13" r:id="rId7"/>
-    <sheet name="get_inception" sheetId="14" r:id="rId8"/>
-    <sheet name="set_title" sheetId="25" r:id="rId9"/>
-    <sheet name="set_author" sheetId="26" r:id="rId10"/>
-    <sheet name="set_param" sheetId="27" r:id="rId11"/>
-    <sheet name="get_param" sheetId="28" r:id="rId12"/>
-    <sheet name="add_interface" sheetId="29" r:id="rId13"/>
-    <sheet name="get_interface" sheetId="30" r:id="rId14"/>
-    <sheet name="get_port" sheetId="31" r:id="rId15"/>
-    <sheet name="add_module" sheetId="32" r:id="rId16"/>
-    <sheet name="get_module" sheetId="33" r:id="rId17"/>
-    <sheet name="add_code" sheetId="39" r:id="rId18"/>
-    <sheet name="i_set_param" sheetId="34" r:id="rId19"/>
-    <sheet name="i_get_param" sheetId="35" r:id="rId20"/>
-    <sheet name="i_set_port" sheetId="36" r:id="rId21"/>
-    <sheet name="i_get_port" sheetId="37" r:id="rId22"/>
-    <sheet name="i_is_valid" sheetId="38" r:id="rId23"/>
+    <sheet name="apply_code" sheetId="40" r:id="rId5"/>
+    <sheet name="find" sheetId="9" r:id="rId6"/>
+    <sheet name="is_valid" sheetId="10" r:id="rId7"/>
+    <sheet name="set_inception" sheetId="13" r:id="rId8"/>
+    <sheet name="get_inception" sheetId="14" r:id="rId9"/>
+    <sheet name="set_title" sheetId="25" r:id="rId10"/>
+    <sheet name="set_author" sheetId="26" r:id="rId11"/>
+    <sheet name="set_param" sheetId="27" r:id="rId12"/>
+    <sheet name="get_param" sheetId="28" r:id="rId13"/>
+    <sheet name="add_interface" sheetId="29" r:id="rId14"/>
+    <sheet name="get_interface" sheetId="30" r:id="rId15"/>
+    <sheet name="get_port" sheetId="31" r:id="rId16"/>
+    <sheet name="add_module" sheetId="32" r:id="rId17"/>
+    <sheet name="get_module" sheetId="33" r:id="rId18"/>
+    <sheet name="add_code" sheetId="39" r:id="rId19"/>
+    <sheet name="i_set_param" sheetId="34" r:id="rId20"/>
+    <sheet name="i_get_param" sheetId="35" r:id="rId21"/>
+    <sheet name="i_set_port" sheetId="36" r:id="rId22"/>
+    <sheet name="i_get_port" sheetId="37" r:id="rId23"/>
+    <sheet name="i_is_valid" sheetId="38" r:id="rId24"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="135">
   <si>
     <t>표현식</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -593,6 +594,27 @@
   <si>
     <t>사용자 코드 추가합니다.
 이 코드들은 각 모듈 소스의 맨 마지막에 삽입되는 문장으로 포함됩니다. module.code(String) 객체에 추가되며, _V() 메크로 함수와 함께 유용하게 사용될 수 있습니다. 추가된 코드의 마지막 문자가 ';' 로 끝날 경우 자동으로 enter code가 삽입됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>code 파일을 module 에 적용합니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.apply_code</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코드 기술 파일로부터 코드를 읽어 각 module 에 코드로 삽입합니다.
+코드 기술 파일에서 ":모듈명" 으로 시작한 뒤, 다음 줄부터 해당 모듈에 코드가 삽입됩니다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function module.apply_code(filename)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코드 기술 파일명</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -928,10 +950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1552F-D2B8-4AD9-9ECE-3CAF9162E459}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1129,12 +1151,23 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
         <v>57</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C19" t="s">
         <v>125</v>
       </c>
     </row>
@@ -1146,6 +1179,59 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4872EA8D-C206-4975-8F57-5608D1E780D6}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B50024F-C566-4A8D-B5DE-B9604581D8DC}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1198,7 +1284,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{928081EA-571E-4518-9D8A-1567A1472513}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -1267,7 +1353,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD855936-E57A-4AAE-A547-E3F2DF4F0374}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1320,7 +1406,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D7D268-AD21-44BB-8182-E394A1BAB6BC}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1381,7 +1467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5785E4B8-2D74-44E5-B491-19BF525ABA02}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1434,7 +1520,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA580444-854B-4B19-9F3C-A3C0598A14F6}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1486,7 +1572,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E82B7A0-A94F-47BE-ACEE-BBB2DA8903FA}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1547,7 +1633,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01B9B674-2006-4921-91E8-F776B72473CB}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1600,11 +1686,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28113802-B713-49E4-A818-7E4C797F3E8E}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1649,67 +1735,6 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A772622C-72EA-4547-94FE-9EA66C7FB6BE}">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="55.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="B5" t="s">
-        <v>109</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1800,6 +1825,67 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A772622C-72EA-4547-94FE-9EA66C7FB6BE}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B5" t="s">
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F508A2DE-DD70-49F7-944A-ED879E70751B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1852,7 +1938,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1F942EC-D9CE-4518-8AE9-9DD2A68C7F6E}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -1913,7 +1999,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3433696-309F-48A2-94BE-A5A058FB822B}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -1966,7 +2052,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F1D0C89-3871-4B99-A935-D12B0A533798}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2084,7 +2170,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -2128,10 +2214,69 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74775AB0-90E6-4F96-93BF-E413632C7F79}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.125" customWidth="1"/>
+    <col min="2" max="2" width="55.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="66" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3BDBF1A7-2EF9-4A6E-97F7-6E6DC3263962}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2191,7 +2336,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB28CFE9-CB71-4320-83F8-E42AFA068774}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -2251,7 +2396,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4066CFF-428B-4723-A23B-AA045754B767}">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -2320,7 +2465,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D19B922-7931-4B59-9944-8B3AC4588909}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -2371,57 +2516,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4872EA8D-C206-4975-8F57-5608D1E780D6}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="10.125" customWidth="1"/>
-    <col min="2" max="2" width="55.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
verigen : add_interface에 modport 를 지정할 수 있게 수정
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_module.xlsx
+++ b/Common/doc/verigen/media/instruction_module.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{276A410C-B576-4CBD-976C-2E3B7DCB086E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F821DFD3-E1D7-40E4-A288-A7C4EA9035E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6000" yWindow="330" windowWidth="18390" windowHeight="15300" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="28830" windowHeight="12150" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="137">
   <si>
     <t>표현식</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -426,10 +426,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>function module:add_interface(i, name)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>interface_i</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -439,10 +435,6 @@
   </si>
   <si>
     <t>interface 객체</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>interface instance 명</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -615,6 +607,24 @@
   </si>
   <si>
     <t>코드 기술 파일명</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>modport 이름, port가 아닌 내부 선언용으로 사용할 경우.
+이 값을 지정하지 않는다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>function module:add_interface(i, [name], [modport])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interface instance 명
+이름을 지정하지 않을 경우 인터페이스 명을 따른다.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1118,13 +1128,13 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1151,13 +1161,13 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C18" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1165,10 +1175,10 @@
         <v>57</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
   </sheetData>
@@ -1408,10 +1418,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D7D268-AD21-44BB-8182-E394A1BAB6BC}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1425,7 +1435,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1433,7 +1443,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1441,23 +1451,31 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B4" t="s">
         <v>90</v>
       </c>
-      <c r="B4" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>92</v>
+      <c r="B5" s="2" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="33" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1486,7 +1504,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1494,7 +1512,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1502,7 +1520,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1510,7 +1528,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1539,7 +1557,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1547,7 +1565,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="33" x14ac:dyDescent="0.3">
@@ -1555,7 +1573,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1563,7 +1581,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1591,7 +1609,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1612,10 +1630,10 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>99</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="66" x14ac:dyDescent="0.3">
@@ -1623,7 +1641,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -1652,7 +1670,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1668,7 +1686,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1676,7 +1694,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1705,7 +1723,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1721,15 +1739,15 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -1843,7 +1861,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1859,7 +1877,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1872,10 +1890,10 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s">
         <v>107</v>
-      </c>
-      <c r="B5" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1904,7 +1922,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1920,7 +1938,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1957,7 +1975,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1973,7 +1991,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1981,15 +1999,15 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B5" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
   </sheetData>
@@ -2018,7 +2036,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2026,7 +2044,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2034,7 +2052,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2042,7 +2060,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
@@ -2071,7 +2089,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -2087,7 +2105,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2095,7 +2113,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -2222,7 +2240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74775AB0-90E6-4F96-93BF-E413632C7F79}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2243,7 +2261,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2259,7 +2277,7 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2267,7 +2285,7 @@
         <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
verigen : 코드 기술에 option 을 추가
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_module.xlsx
+++ b/Common/doc/verigen/media/instruction_module.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F821DFD3-E1D7-40E4-A288-A7C4EA9035E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5717D87B-5733-46A6-B54F-6C5F8E031648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="390" windowWidth="28830" windowHeight="12150" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="390" windowWidth="28830" windowHeight="12150" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -597,11 +597,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>코드 기술 파일로부터 코드를 읽어 각 module 에 코드로 삽입합니다.
-코드 기술 파일에서 ":모듈명" 으로 시작한 뒤, 다음 줄부터 해당 모듈에 코드가 삽입됩니다.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>function module.apply_code(filename)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -625,6 +620,12 @@
   <si>
     <t>interface instance 명
 이름을 지정하지 않을 경우 인터페이스 명을 따른다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>코드 기술 파일로부터 코드를 읽어 각 module 에 코드로 삽입합니다.
+코드 기술 파일에서 ":모듈명 (옵션)" 으로 시작한 뒤, 다음 줄부터 해당 모듈에 코드가 옵션의 결과가 true 일 때, 삽입됩니다.
+옵션은 하위 기술된 코드들이 삽입 여부를 나타내는 Boolean 결과의 Lua 스크립트입니다. 이 옵션은 생략될 수 있습니다. (기본 값 : true)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1420,7 +1421,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D7D268-AD21-44BB-8182-E394A1BAB6BC}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1435,7 +1436,7 @@
         <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1467,15 +1468,15 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="33" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2240,7 +2241,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74775AB0-90E6-4F96-93BF-E413632C7F79}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2261,7 +2264,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -2272,12 +2275,12 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="66" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" ht="115.5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2285,7 +2288,7 @@
         <v>66</v>
       </c>
       <c r="B5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
verigen 의 module:add_interface 사용성 개선
</commit_message>
<xml_diff>
--- a/Common/doc/verigen/media/instruction_module.xlsx
+++ b/Common/doc/verigen/media/instruction_module.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\Profiles\Common\doc\verigen\media\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E010502F-4C6A-46C2-B28F-701D3E472890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84998DF-61D4-40B6-9866-469A162A8082}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="300" windowWidth="21405" windowHeight="15405" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4380" yWindow="2175" windowWidth="21465" windowHeight="13425" firstSheet="10" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="6" r:id="rId1"/>
@@ -544,17 +544,8 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>interface object</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>interface instance name
 If the name is not specified, the interface name is followed.</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>The modport name, if used for internal declarations other than ports.
-Do not specify this value.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -668,6 +659,15 @@
   </si>
   <si>
     <t>Add a document.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>interface object or interface modeport</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The modport name, if used for internal declarations other than ports.
+Do not specify this value. And if 'I' is modport, then this 'modport must be nil.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1005,7 +1005,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63D1552F-D2B8-4AD9-9ECE-3CAF9162E459}">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
@@ -1193,13 +1193,13 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1280,7 +1280,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1296,7 +1296,7 @@
         <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1304,7 +1304,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="66" x14ac:dyDescent="0.3">
@@ -1312,7 +1312,7 @@
         <v>32</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
   </sheetData>
@@ -1586,7 +1586,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3D7D268-AD21-44BB-8182-E394A1BAB6BC}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -1633,7 +1633,7 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>117</v>
+        <v>145</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="33" x14ac:dyDescent="0.3">
@@ -1641,15 +1641,15 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="49.5" x14ac:dyDescent="0.3">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="66" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>119</v>
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -1702,7 +1702,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1710,7 +1710,7 @@
         <v>65</v>
       </c>
       <c r="B5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -1762,7 +1762,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1770,7 +1770,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1823,7 +1823,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1831,7 +1831,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -1892,7 +1892,7 @@
         <v>46</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="82.5" x14ac:dyDescent="0.3">
@@ -1900,7 +1900,7 @@
         <v>0</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>
@@ -2050,7 +2050,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2058,7 +2058,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -2111,7 +2111,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2119,7 +2119,7 @@
         <v>58</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -2171,7 +2171,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2187,7 +2187,7 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -2240,7 +2240,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2301,7 +2301,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2309,7 +2309,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -2317,7 +2317,7 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -2362,7 +2362,7 @@
         <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -2370,7 +2370,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2378,7 +2378,7 @@
         <v>0</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -2431,7 +2431,7 @@
         <v>68</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -2439,7 +2439,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>